<commit_message>
Gitignore file slightly updated
</commit_message>
<xml_diff>
--- a/src/main/resources/TestOutPut.xlsx
+++ b/src/main/resources/TestOutPut.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="SortBy" sheetId="1" r:id="rId1"/>
@@ -39,10 +39,10 @@
     <t>$73.00 - $210.32</t>
   </si>
   <si>
-    <t>$92.00 - $252.75</t>
-  </si>
-  <si>
-    <t>658.63</t>
+    <t>$91.00 - $252.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 73 00-</t>
   </si>
   <si>
     <t>$85.99 - $155.00</t>
@@ -54,8 +54,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -89,7 +88,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -97,14 +96,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -142,9 +144,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -179,7 +181,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -214,7 +216,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -388,25 +390,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="14.77734375" collapsed="true"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -414,7 +413,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -422,7 +421,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -430,7 +429,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -438,7 +437,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -458,7 +457,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -470,7 +469,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>